<commit_message>
Update crew configurations and clean up output files
- Updated excel_processor and email_builder crew configs
- Cleaned up generated output files
- Updated plan documentation

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/input/TBS Price Change Summary Report - October 13th'25.xlsx
+++ b/data/input/TBS Price Change Summary Report - October 13th'25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://anheuserbuschinbev-my.sharepoint.com/personal/aaditya_singhal_anheuser-busch_com/Documents/FY25/Personal git repo/RevMan-POC-Crew/revman/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{0AA89260-8720-4988-BC56-22AC02704366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7723D4F6-A632-4E6A-B77F-EB0EB3408CA2}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{0AA89260-8720-4988-BC56-22AC02704366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62131F4D-22FA-4E72-A89A-9E537196FD15}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6A2125F1-4E47-4331-8639-117622155337}"/>
   </bookViews>
@@ -9038,6 +9038,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A8:L190" xr:uid="{F88453A7-FECA-4927-826D-F01BE31EC038}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:K190">
     <sortCondition ref="C9:C190"/>
     <sortCondition ref="D9:D190"/>
@@ -9064,15 +9065,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003BD24DCF8EBA2A459A3767B75ECBC810" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="14ba1abd425e7d287f53e65cd7fdc17f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4d19c67b-01ac-4d4b-a843-fb81d321b596" xmlns:ns3="6dca17fb-ac11-4cf8-b45b-b93bf268ff03" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f877f0b356da1ae16043b73a66e5efc3" ns2:_="" ns3:_="">
     <xsd:import namespace="4d19c67b-01ac-4d4b-a843-fb81d321b596"/>
@@ -9327,6 +9319,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -9339,14 +9340,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B6DF62D-6E20-4488-8172-8E2FED293569}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{663EA9A2-C52A-4722-944D-0B4351AA8E9D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9365,6 +9358,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B6DF62D-6E20-4488-8172-8E2FED293569}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E560CAD-3D0D-4622-8ACC-0E2F5560BCED}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Refine crew configurations and improve flow orchestration
- Simplify plan.md and align with current implementation
- Update Excel processor crew agents and tasks for better task chaining
- Update Email builder crew tasks for structured output
- Improve main.py flow with better error handling and validation
- Remove unused email_tools.py module
- Clean up excel_tools.py imports

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/input/TBS Price Change Summary Report - October 13th'25.xlsx
+++ b/data/input/TBS Price Change Summary Report - October 13th'25.xlsx
@@ -1072,7 +1072,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="R33" sqref="R33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="10"/>
@@ -9065,6 +9065,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003BD24DCF8EBA2A459A3767B75ECBC810" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="14ba1abd425e7d287f53e65cd7fdc17f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4d19c67b-01ac-4d4b-a843-fb81d321b596" xmlns:ns3="6dca17fb-ac11-4cf8-b45b-b93bf268ff03" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f877f0b356da1ae16043b73a66e5efc3" ns2:_="" ns3:_="">
     <xsd:import namespace="4d19c67b-01ac-4d4b-a843-fb81d321b596"/>
@@ -9319,15 +9328,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -9340,6 +9340,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B6DF62D-6E20-4488-8172-8E2FED293569}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{663EA9A2-C52A-4722-944D-0B4351AA8E9D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9358,14 +9366,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B6DF62D-6E20-4488-8172-8E2FED293569}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E560CAD-3D0D-4622-8ACC-0E2F5560BCED}">
   <ds:schemaRefs>

</xml_diff>